<commit_message>
Remove 2026-02-13 data & update schedule to 20:45
</commit_message>
<xml_diff>
--- a/理想南向持有.xlsx
+++ b/理想南向持有.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>日期</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>2026-02-12</t>
-  </si>
-  <si>
-    <t>2026-02-13</t>
   </si>
 </sst>
 </file>
@@ -602,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1422,17 +1419,6 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>76</v>
-      </c>
-      <c r="B75">
-        <v>42.53</v>
-      </c>
-      <c r="C75">
-        <v>5.29754581</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>